<commit_message>
added rev 3 dxf to the normal sized maser copy
</commit_message>
<xml_diff>
--- a/normal sized ultimaker files/cut sheets/parts list for regular sized machine.xlsx
+++ b/normal sized ultimaker files/cut sheets/parts list for regular sized machine.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Qty.</t>
   </si>
@@ -46,9 +46,6 @@
     <t>8mm linear bearings</t>
   </si>
   <si>
-    <t>M3 x 10 screw</t>
-  </si>
-  <si>
     <t>M3 x 15 screw</t>
   </si>
   <si>
@@ -61,15 +58,9 @@
     <t>M3 x 30</t>
   </si>
   <si>
-    <t>Normal nuts</t>
-  </si>
-  <si>
     <t>tight locking nuts M3</t>
   </si>
   <si>
-    <t>Square nuts</t>
-  </si>
-  <si>
     <t>spacer pack v1</t>
   </si>
   <si>
@@ -94,26 +85,83 @@
     <t>Supplier</t>
   </si>
   <si>
-    <t>SDP/SI?</t>
-  </si>
-  <si>
     <t>3 X</t>
   </si>
   <si>
     <t xml:space="preserve">1 x </t>
   </si>
   <si>
-    <t>36 inch long 8mm smooth rods?</t>
-  </si>
-  <si>
-    <t>36 inch long 12mm smooth rod?</t>
+    <t>peek insulator</t>
+  </si>
+  <si>
+    <t>5mm to 8mm shaft coupling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFA tubing possible 1/4" or 3.18mm id 6.35mm od 1.6mm wall </t>
+  </si>
+  <si>
+    <t>http://www.freshwatersystems.com/p-1432-straight-bspt-male-14-push-in-x-18-bspt.aspx</t>
+  </si>
+  <si>
+    <t>M3 hex nuts</t>
+  </si>
+  <si>
+    <t>econobelt</t>
+  </si>
+  <si>
+    <t>nema 17 stepper motors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 x 10 screw </t>
+  </si>
+  <si>
+    <t>3mm tumb screw knob for a 3mm screw</t>
+  </si>
+  <si>
+    <t>M8 threaded rod for z axis</t>
+  </si>
+  <si>
+    <t>1x</t>
+  </si>
+  <si>
+    <t>extruder parts</t>
+  </si>
+  <si>
+    <t>DMfit Straight BSPT Male - 1/4" Push-in x 1/8" BSPT(alt use watts pl3004 from lowes</t>
+  </si>
+  <si>
+    <t>watts collet clip 3547B-08</t>
+  </si>
+  <si>
+    <t>watts 1/4 inch push fitting line crimp remove from fitting or watts 159B-08</t>
+  </si>
+  <si>
+    <t>mcmaster carr</t>
+  </si>
+  <si>
+    <t>http://www.huronindustrial.com/mm5/merchant.mvc?Screen=PROD&amp;Store_Code=his&amp;Product_Code=1-950M-008&amp;Category_Code=</t>
+  </si>
+  <si>
+    <t>36 inch long 8mm smooth rods? Oil hardened 0-1 8mm drill rod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 inch long 12mm smooth rod? </t>
+  </si>
+  <si>
+    <t>4.54 each</t>
+  </si>
+  <si>
+    <t>http://www.huronindustrial.com/mm5/merchant.mvc?Screen=PROD&amp;Store_Code=his&amp;Product_Code=1-950M-012&amp;Category_Code=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +174,28 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,17 +215,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,18 +527,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="122" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,45 +548,54 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -513,10 +603,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -524,7 +614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -532,7 +622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -540,105 +630,197 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="6">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6">
+        <v>9.6199999999999992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>11</v>
+      </c>
+      <c r="D14" s="6">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="D15" s="6">
+        <v>6.55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>28</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>60</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="6">
+        <v>9.4700000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="B31" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="B32" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C32" r:id="rId1"/>
+    <hyperlink ref="C22" r:id="rId2"/>
+    <hyperlink ref="C23" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added a bunch of .dxf drawings of the parts that need to be machined and the electronic scmatics
</commit_message>
<xml_diff>
--- a/normal sized ultimaker files/cut sheets/parts list for regular sized machine.xlsx
+++ b/normal sized ultimaker files/cut sheets/parts list for regular sized machine.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Qty.</t>
   </si>
@@ -33,125 +33,131 @@
     <t>4x</t>
   </si>
   <si>
+    <t>688 ball bearings (8mm ID, double sealed)</t>
+  </si>
+  <si>
+    <t>brass bushings</t>
+  </si>
+  <si>
+    <t>M3 x 15 screw</t>
+  </si>
+  <si>
+    <t>M3 x 20</t>
+  </si>
+  <si>
+    <t>M3 x 25</t>
+  </si>
+  <si>
+    <t>M3 x 30</t>
+  </si>
+  <si>
+    <t>tight locking nuts M3</t>
+  </si>
+  <si>
+    <t>spacer pack v1</t>
+  </si>
+  <si>
+    <t>washers (new)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 mm ID Pulley 20 tooth MXL </t>
+  </si>
+  <si>
+    <t>5 mm ID pulley 20 tooth MXL</t>
+  </si>
+  <si>
+    <t>short timing belts 100MXL (97MXL?)</t>
+  </si>
+  <si>
+    <t>long timing belt 300MXL (295MXL?)</t>
+  </si>
+  <si>
+    <t>VBX?</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>3 X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x </t>
+  </si>
+  <si>
+    <t>peek insulator</t>
+  </si>
+  <si>
+    <t>5mm to 8mm shaft coupling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFA tubing possible 1/4" or 3.18mm id 6.35mm od 1.6mm wall </t>
+  </si>
+  <si>
+    <t>http://www.freshwatersystems.com/p-1432-straight-bspt-male-14-push-in-x-18-bspt.aspx</t>
+  </si>
+  <si>
+    <t>M3 hex nuts</t>
+  </si>
+  <si>
+    <t>econobelt</t>
+  </si>
+  <si>
+    <t>nema 17 stepper motors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 x 10 screw </t>
+  </si>
+  <si>
+    <t>3mm tumb screw knob for a 3mm screw</t>
+  </si>
+  <si>
+    <t>1x</t>
+  </si>
+  <si>
+    <t>extruder parts</t>
+  </si>
+  <si>
+    <t>DMfit Straight BSPT Male - 1/4" Push-in x 1/8" BSPT(alt use watts pl3004 from lowes</t>
+  </si>
+  <si>
+    <t>watts collet clip 3547B-08</t>
+  </si>
+  <si>
+    <t>watts 1/4 inch push fitting line crimp remove from fitting or watts 159B-08</t>
+  </si>
+  <si>
+    <t>mcmaster carr</t>
+  </si>
+  <si>
+    <t>http://www.huronindustrial.com/mm5/merchant.mvc?Screen=PROD&amp;Store_Code=his&amp;Product_Code=1-950M-008&amp;Category_Code=</t>
+  </si>
+  <si>
+    <t>36 inch long 8mm smooth rods? Oil hardened 0-1 8mm drill rod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 inch long 12mm smooth rod? </t>
+  </si>
+  <si>
+    <t>4.54 each</t>
+  </si>
+  <si>
+    <t>http://www.huronindustrial.com/mm5/merchant.mvc?Screen=PROD&amp;Store_Code=his&amp;Product_Code=1-950M-012&amp;Category_Code=</t>
+  </si>
+  <si>
+    <t>8mm linear bearings these are lm8luu and are longer bearings I found these on ebay</t>
+  </si>
+  <si>
     <t>Large linear bearings
-(12mm internal diameter)</t>
-  </si>
-  <si>
-    <t>688 ball bearings (8mm ID, double sealed)</t>
-  </si>
-  <si>
-    <t>brass bushings</t>
-  </si>
-  <si>
-    <t>8mm linear bearings</t>
-  </si>
-  <si>
-    <t>M3 x 15 screw</t>
-  </si>
-  <si>
-    <t>M3 x 20</t>
-  </si>
-  <si>
-    <t>M3 x 25</t>
-  </si>
-  <si>
-    <t>M3 x 30</t>
-  </si>
-  <si>
-    <t>tight locking nuts M3</t>
-  </si>
-  <si>
-    <t>spacer pack v1</t>
-  </si>
-  <si>
-    <t>washers (new)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 mm ID Pulley 20 tooth MXL </t>
-  </si>
-  <si>
-    <t>5 mm ID pulley 20 tooth MXL</t>
-  </si>
-  <si>
-    <t>short timing belts 100MXL (97MXL?)</t>
-  </si>
-  <si>
-    <t>long timing belt 300MXL (295MXL?)</t>
-  </si>
-  <si>
-    <t>VBX?</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>3 X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x </t>
-  </si>
-  <si>
-    <t>peek insulator</t>
-  </si>
-  <si>
-    <t>5mm to 8mm shaft coupling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PFA tubing possible 1/4" or 3.18mm id 6.35mm od 1.6mm wall </t>
-  </si>
-  <si>
-    <t>http://www.freshwatersystems.com/p-1432-straight-bspt-male-14-push-in-x-18-bspt.aspx</t>
-  </si>
-  <si>
-    <t>M3 hex nuts</t>
-  </si>
-  <si>
-    <t>econobelt</t>
-  </si>
-  <si>
-    <t>nema 17 stepper motors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3 x 10 screw </t>
-  </si>
-  <si>
-    <t>3mm tumb screw knob for a 3mm screw</t>
-  </si>
-  <si>
-    <t>M8 threaded rod for z axis</t>
-  </si>
-  <si>
-    <t>1x</t>
-  </si>
-  <si>
-    <t>extruder parts</t>
-  </si>
-  <si>
-    <t>DMfit Straight BSPT Male - 1/4" Push-in x 1/8" BSPT(alt use watts pl3004 from lowes</t>
-  </si>
-  <si>
-    <t>watts collet clip 3547B-08</t>
-  </si>
-  <si>
-    <t>watts 1/4 inch push fitting line crimp remove from fitting or watts 159B-08</t>
-  </si>
-  <si>
-    <t>mcmaster carr</t>
-  </si>
-  <si>
-    <t>http://www.huronindustrial.com/mm5/merchant.mvc?Screen=PROD&amp;Store_Code=his&amp;Product_Code=1-950M-008&amp;Category_Code=</t>
-  </si>
-  <si>
-    <t>36 inch long 8mm smooth rods? Oil hardened 0-1 8mm drill rod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36 inch long 12mm smooth rod? </t>
-  </si>
-  <si>
-    <t>4.54 each</t>
-  </si>
-  <si>
-    <t>http://www.huronindustrial.com/mm5/merchant.mvc?Screen=PROD&amp;Store_Code=his&amp;Product_Code=1-950M-012&amp;Category_Code=</t>
+(12mm internal diameter) lm12luu</t>
+  </si>
+  <si>
+    <t>M12x3 acme threaded rod for z axis</t>
+  </si>
+  <si>
+    <t>acme nut 12mmx3 7549k33 grind flat on 2 sides to 18mm wide</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#metric-acme-nuts/=ez8424</t>
   </si>
 </sst>
 </file>
@@ -529,13 +535,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="122" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
@@ -548,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -556,10 +562,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -567,10 +573,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -578,10 +584,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -589,10 +595,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30">
@@ -600,10 +606,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -611,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -619,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -627,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -635,10 +641,10 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D11" s="6">
         <v>8.3800000000000008</v>
@@ -649,7 +655,7 @@
         <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" s="6">
         <v>9.6199999999999992</v>
@@ -660,7 +666,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="6">
         <v>6.02</v>
@@ -671,7 +677,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="6">
         <v>6.13</v>
@@ -682,7 +688,7 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="6">
         <v>6.55</v>
@@ -693,7 +699,7 @@
         <v>180</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="6">
         <v>2</v>
@@ -704,7 +710,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -712,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -720,32 +726,32 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D23" s="6">
         <v>9.4700000000000006</v>
@@ -753,15 +759,29 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="6">
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -769,12 +789,12 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -782,35 +802,35 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -818,9 +838,10 @@
     <hyperlink ref="C32" r:id="rId1"/>
     <hyperlink ref="C22" r:id="rId2"/>
     <hyperlink ref="C23" r:id="rId3"/>
+    <hyperlink ref="C25" r:id="rId4" location="metric-acme-nuts/=ez8424" display="http://www.mcmaster.com/ - metric-acme-nuts/=ez8424"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
found some more parts!!
</commit_message>
<xml_diff>
--- a/normal sized ultimaker files/cut sheets/parts list for regular sized machine.xlsx
+++ b/normal sized ultimaker files/cut sheets/parts list for regular sized machine.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Qty.</t>
   </si>
@@ -87,9 +87,6 @@
     <t>peek insulator</t>
   </si>
   <si>
-    <t>5mm to 8mm shaft coupling</t>
-  </si>
-  <si>
     <t xml:space="preserve">PFA tubing possible 1/4" or 3.18mm id 6.35mm od 1.6mm wall </t>
   </si>
   <si>
@@ -136,9 +133,6 @@
   </si>
   <si>
     <t xml:space="preserve">36 inch long 12mm smooth rod? </t>
-  </si>
-  <si>
-    <t>4.54 each</t>
   </si>
   <si>
     <t>http://www.huronindustrial.com/mm5/merchant.mvc?Screen=PROD&amp;Store_Code=his&amp;Product_Code=1-950M-012&amp;Category_Code=</t>
@@ -158,6 +152,12 @@
   </si>
   <si>
     <t>http://www.mcmaster.com/#metric-acme-nuts/=ez8424</t>
+  </si>
+  <si>
+    <t>5mm to 8mm shaft coupling sdp-si part# S51CAYM050080</t>
+  </si>
+  <si>
+    <t>https://sdp-si.com/eStore/</t>
   </si>
 </sst>
 </file>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,7 +565,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -576,7 +576,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -587,7 +587,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -598,7 +598,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30">
@@ -606,7 +606,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -633,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -641,10 +641,10 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="6">
         <v>8.3800000000000008</v>
@@ -699,7 +699,7 @@
         <v>180</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="6">
         <v>2</v>
@@ -734,13 +734,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="D22" s="6">
+        <v>13.62</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -748,10 +748,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D23" s="6">
         <v>9.4700000000000006</v>
@@ -759,29 +759,38 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D25" s="6">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="6">
+        <v>16.68</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -789,12 +798,12 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -802,15 +811,15 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="2:2">
@@ -820,17 +829,17 @@
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -839,9 +848,10 @@
     <hyperlink ref="C22" r:id="rId2"/>
     <hyperlink ref="C23" r:id="rId3"/>
     <hyperlink ref="C25" r:id="rId4" location="metric-acme-nuts/=ez8424" display="http://www.mcmaster.com/ - metric-acme-nuts/=ez8424"/>
+    <hyperlink ref="C27" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
made some more changes to the files and removed all of the as220 cust so i can remoke them again
</commit_message>
<xml_diff>
--- a/normal sized ultimaker files/cut sheets/parts list for regular sized machine.xlsx
+++ b/normal sized ultimaker files/cut sheets/parts list for regular sized machine.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Qty.</t>
   </si>
@@ -39,18 +39,6 @@
     <t>brass bushings</t>
   </si>
   <si>
-    <t>M3 x 15 screw</t>
-  </si>
-  <si>
-    <t>M3 x 20</t>
-  </si>
-  <si>
-    <t>M3 x 25</t>
-  </si>
-  <si>
-    <t>M3 x 30</t>
-  </si>
-  <si>
     <t>tight locking nuts M3</t>
   </si>
   <si>
@@ -60,12 +48,6 @@
     <t>washers (new)</t>
   </si>
   <si>
-    <t xml:space="preserve">8 mm ID Pulley 20 tooth MXL </t>
-  </si>
-  <si>
-    <t>5 mm ID pulley 20 tooth MXL</t>
-  </si>
-  <si>
     <t>short timing belts 100MXL (97MXL?)</t>
   </si>
   <si>
@@ -93,16 +75,7 @@
     <t>http://www.freshwatersystems.com/p-1432-straight-bspt-male-14-push-in-x-18-bspt.aspx</t>
   </si>
   <si>
-    <t>M3 hex nuts</t>
-  </si>
-  <si>
-    <t>econobelt</t>
-  </si>
-  <si>
     <t>nema 17 stepper motors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3 x 10 screw </t>
   </si>
   <si>
     <t>3mm tumb screw knob for a 3mm screw</t>
@@ -158,6 +131,36 @@
   </si>
   <si>
     <t>https://sdp-si.com/eStore/</t>
+  </si>
+  <si>
+    <t>8 mm ID Pulley 20 tooth MXL QPMMXLA25020F04</t>
+  </si>
+  <si>
+    <t>5 mm ID pulley 20 tooth MXL QPMMXLA25020F04</t>
+  </si>
+  <si>
+    <t>http://www.econobelt.com/Q460/RFQ/default.asp?Page=Pg_1-004_1.html</t>
+  </si>
+  <si>
+    <t>http://www.econobelt.com/Q460/RFQ/default.asp?Page=tbelt/02.htm</t>
+  </si>
+  <si>
+    <t>M3 x 10 screw  PN#92095A177</t>
+  </si>
+  <si>
+    <t>M3 x 16 screw PN#92095A184</t>
+  </si>
+  <si>
+    <t>M3 x 20 PN#92095A185</t>
+  </si>
+  <si>
+    <t>M3 x 25 PN#92095A186</t>
+  </si>
+  <si>
+    <t>M3 x 30 PN#92095A187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 hex nuts </t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -554,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -562,10 +565,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="6">
+        <v>59.8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -573,10 +579,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6">
+        <v>11.96</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -584,10 +593,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="6">
+        <v>8.84</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -595,10 +607,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4.24</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30">
@@ -606,10 +621,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -633,7 +648,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -641,10 +656,10 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D11" s="6">
         <v>8.3800000000000008</v>
@@ -655,7 +670,7 @@
         <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D12" s="6">
         <v>9.6199999999999992</v>
@@ -666,7 +681,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D13" s="6">
         <v>6.02</v>
@@ -677,7 +692,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D14" s="6">
         <v>6.13</v>
@@ -688,7 +703,7 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D15" s="6">
         <v>6.55</v>
@@ -699,7 +714,7 @@
         <v>180</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D16" s="6">
         <v>2</v>
@@ -710,7 +725,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -718,7 +733,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -726,18 +741,18 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D22" s="6">
         <v>13.62</v>
@@ -745,13 +760,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D23" s="6">
         <v>9.4700000000000006</v>
@@ -759,21 +774,21 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D25" s="6">
         <v>29</v>
@@ -781,13 +796,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D27" s="6">
         <v>16.68</v>
@@ -798,12 +813,12 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -811,35 +826,46 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" t="s">
-        <v>33</v>
+    <row r="38" spans="2:4">
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="D39" s="6">
+        <f>SUM(D2:D38)</f>
+        <v>192.30999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -849,9 +875,13 @@
     <hyperlink ref="C23" r:id="rId3"/>
     <hyperlink ref="C25" r:id="rId4" location="metric-acme-nuts/=ez8424" display="http://www.mcmaster.com/ - metric-acme-nuts/=ez8424"/>
     <hyperlink ref="C27" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="C3" r:id="rId7"/>
+    <hyperlink ref="C4" r:id="rId8"/>
+    <hyperlink ref="C5" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>